<commit_message>
weight align fed learning
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewgorbett/PycharmProjects/iterative_weight_alignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F684B5-71A2-9044-8029-286F9C8BD951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8651CDA-16B5-504B-A672-22113277FADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="500" windowWidth="28040" windowHeight="18200" xr2:uid="{594364FA-10F3-764D-A9C9-CB98B77E52EF}"/>
+    <workbookView xWindow="2760" yWindow="500" windowWidth="28040" windowHeight="18200" xr2:uid="{594364FA-10F3-764D-A9C9-CB98B77E52EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2292B53-1D3E-0E46-9B24-D0A3A204ABAD}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,44 +532,27 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -589,7 +572,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -609,7 +592,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -620,13 +603,16 @@
       <c r="D12" t="s">
         <v>8</v>
       </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
       <c r="G12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -641,35 +627,32 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -683,13 +666,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -703,16 +686,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
       </c>
       <c r="G19" t="s">
         <v>26</v>
@@ -720,41 +706,41 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B20">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -771,7 +757,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>20</v>
@@ -788,7 +774,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -805,7 +791,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>20</v>
@@ -820,26 +806,26 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
         <v>7</v>
       </c>
-      <c r="D28" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29">
         <v>20</v>
@@ -856,7 +842,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B30">
         <v>20</v>
@@ -873,7 +859,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31">
         <v>20</v>
@@ -890,7 +876,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32">
         <v>20</v>
@@ -902,6 +888,23 @@
         <v>9</v>
       </c>
       <c r="G32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>